<commit_message>
unfinished translations, there is still some left
</commit_message>
<xml_diff>
--- a/Translations/Translations 1.xlsx
+++ b/Translations/Translations 1.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ituniversity-my.sharepoint.com/personal/gifa_itu_dk/Documents/Documents/GitHub/data-wild-west/Translations/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Veronii\Desktop\data-wild-west\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{40D70338-D5F7-42E2-A2A0-77D7B3E0FCF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9ACE8717-E370-4E09-9415-AE7F11B02AB5}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="Trans.1" sheetId="3" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t>Priserne stiger, mens centrene forfalder mere og mere. :( Mange af redskaberne er virkelig slidte og nogen helt ødelagte. Standarden af centrene varierer også en del, hvilket er trist, når man bor tæt på et center, som ikke bliver prioriteret så meget, men stadig betaler det samme…</t>
   </si>
@@ -92,12 +91,36 @@
   </si>
   <si>
     <t>Neg</t>
+  </si>
+  <si>
+    <t>During the time when I was by Sats, the sauna and cold shower were not always functioning. The cables also often break, and it took a long tie before they were fixed. There has been a time of saving, and a tough economy, so it is what it is. It is stil not optimal, though. What is really unfortunate, is that I could not work out anymore, so I wanted to cancel my subscription. Sats offered me 2 months of rest period for free. I accept that. I find out that i cannot work out anyore, so i cancel my subscription. That also means, that the rest period is cancelled, and that I should pay of +1 month as I go from today. Payment as I go plus a month is pretty normal, but that they did not inform me clearly, that the rest period that they offered me would be cancelled disappoints me greatly. I am 20 years old, and have always done sports. After I have finished a marathon in the beginning of November, I will sign up for fitness again. That Sats is is not more transparent, and that their customer support is not helpful, makes them lose a custoer, that had provided them years of income. Edit. I worked out at Noerrebro, so it is possible that other places don't have as many problems.</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>This morning I have unfortunately had a bad experience of your customer service at Jens Baggesensvej in Aarhus. I work out in the morning and I arrive at the gym at 7 o'clock, where I find out I unfortunately have forgotten my card. No problem, I think, because I know there is always staff who clean and put products on shelves etc., who presumably could help poor me. A personal trainer is at the counter and receive my message, and walks down to the staff who are cleaning downstairs. Two minutes later he comes back and informs me, that they unfortunately can't help, since they only serve customers after 8, so I had to wait an hour. I find that to be a terrible experience and I will cancel my subscription because of that. Kind regards, Steffen.</t>
+  </si>
+  <si>
+    <t>Sats Frederiksberg falkoner. Absurdedly bad service the first. Absurd terrible bad customer service and lacking empathy service is the first sentence that I choose to begin this review with. The afternoon wednesdag I meet someone who never says hi or have a good day, She is busy with small talk with her colleague. But i am noticed when i am followed into the changing room, where an employee is walking around and looking, crosses personal boundaries and i think it it bad behaviour, and not the least really bad service. The music is so loud that even with headphones, you can't hear anything but noice and bad music.</t>
+  </si>
+  <si>
+    <t>My favorite gym at nygaardsvej, especially after betine began as gym leader and not the least the staff, they do it really well. Members have to be better at cleaning up after themselves. Eternal problem…:) but the music in the gym is often very very load (at least early in the morning) og it is often hip hop and gangta rap, maybe one should try music that is directed at a wider audience, everyone's wearing headphones anyway, the music can be so loud that you can't your own musik in the headphones and if i talk to the staff, but they are not much for turning it down.</t>
+  </si>
+  <si>
+    <t>After being a customer by sats and always having paid my bills (overpriced) throughout 7 years, I got a new cellphone last month after getting anew job. This meant that my bill was not paid in time -- 100% my fault. The next thing that happens was that SATS sent my to Intrum -- a debt repayment firm of the worst kind. Really disappointed in the treatment from SATS. On the other hand really good to be made aware of how i can use 400 kr every month on a terrible firm :-)</t>
+  </si>
+  <si>
+    <t>I paid for my membership three days ago and I still haven't got my confirmation on my sign up or got my membership activated. This hasn't happened, even though I was assured, that I would be done today, when I called at 8:30. It is already suboptimal, that you have to wait from the payment until the establishment of the membership, but it gives an even worse experience, when something is put in view, which doesn't materialize.</t>
+  </si>
+  <si>
+    <t>You need new machines, it is flooding with paper, the toilets in the locker rooms are disgusting, the dumbbells are placed randomly and sometimes spread out around the gym, other customers almost never put the weights back in place. Apart from the machines, the previously mentioned can be corrected by having demands for the customers. Fx. make a video about good behavior in the gym.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -575,13 +598,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -943,50 +969,50 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="129.7109375" customWidth="1"/>
-    <col min="2" max="2" width="74.28515625" customWidth="1"/>
-    <col min="3" max="12" width="5.7109375" customWidth="1"/>
+    <col min="1" max="1" width="129.703125" customWidth="1"/>
+    <col min="2" max="2" width="74.29296875" style="3" customWidth="1"/>
+    <col min="3" max="12" width="5.703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4" t="s">
+      <c r="D1" s="5"/>
+      <c r="E1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4" t="s">
+      <c r="F1" s="5"/>
+      <c r="G1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4" t="s">
+      <c r="H1" s="5"/>
+      <c r="I1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="4"/>
-      <c r="K1" s="3" t="s">
+      <c r="J1" s="5"/>
+      <c r="K1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="3"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
+      <c r="L1" s="4"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A2" s="5"/>
       <c r="B2" s="4" t="s">
         <v>16</v>
       </c>
@@ -1021,124 +1047,169 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="144.69999999999999" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="156.35" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="144" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="115.7" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="86" x14ac:dyDescent="0.5">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A15" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A16" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A17" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A18" s="2"/>
     </row>
-    <row r="19" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A19" s="2"/>
     </row>
-    <row r="20" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A20" s="2"/>
     </row>
-    <row r="21" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A21" s="2"/>
     </row>
-    <row r="22" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A22" s="2"/>
     </row>
-    <row r="23" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A23" s="2"/>
     </row>
-    <row r="24" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A24" s="2"/>
     </row>
-    <row r="25" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A25" s="2"/>
     </row>
-    <row r="26" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A26" s="2"/>
     </row>
-    <row r="27" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A27" s="2"/>
     </row>
-    <row r="28" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A28" s="2"/>
     </row>
-    <row r="29" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A29" s="2"/>
     </row>
-    <row r="30" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A30" s="2"/>
     </row>
-    <row r="31" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A31" s="2"/>
     </row>
-    <row r="32" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" ht="45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A32" s="2"/>
     </row>
   </sheetData>
@@ -1152,5 +1223,6 @@
     <mergeCell ref="I1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>